<commit_message>
Fixed list duplicates function
</commit_message>
<xml_diff>
--- a/src/confluence/test_files/simple1.xlsx
+++ b/src/confluence/test_files/simple1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/confluence/src/confluence/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41467E36-7115-4C4D-AC4B-5FC1E11AAA75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2F3349-1030-6545-98D7-186355FE6619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2000" windowWidth="15380" windowHeight="8440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -461,6 +461,22 @@
       </c>
       <c r="B3">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed confluence_CLI.py to confluence.py
</commit_message>
<xml_diff>
--- a/src/confluence/test_files/simple1.xlsx
+++ b/src/confluence/test_files/simple1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/confluence/src/confluence/test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorweddle/Research/confluence/src/confluence/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2F3349-1030-6545-98D7-186355FE6619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05799A74-C40D-804C-B0D5-C37FE1924598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2000" windowWidth="15380" windowHeight="8440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,10 +23,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>foo</t>
+    <t>bar</t>
   </si>
   <si>
-    <t>bar</t>
+    <t>Sample Name</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -439,12 +439,12 @@
     <col min="1" max="2" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="69" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -465,7 +465,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>3</v>

</xml_diff>